<commit_message>
jenkins icin degidiklik yapildi.
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/resource/ScenarioStatus.xlsx
+++ b/src/test/java/ApachePOI/resource/ScenarioStatus.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="20">
   <si>
     <t>Create a country</t>
   </si>
@@ -74,6 +74,12 @@
   </si>
   <si>
     <t>03.10.22</t>
+  </si>
+  <si>
+    <t>12.10.22</t>
+  </si>
+  <si>
+    <t>Create a country  with parameter data</t>
   </si>
 </sst>
 </file>
@@ -426,7 +432,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D70"/>
+  <dimension ref="A1:D72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
@@ -1418,6 +1424,34 @@
         <v>17</v>
       </c>
     </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>0</v>
+      </c>
+      <c r="B71" t="s">
+        <v>1</v>
+      </c>
+      <c r="C71" t="s">
+        <v>2</v>
+      </c>
+      <c r="D71" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>19</v>
+      </c>
+      <c r="B72" t="s">
+        <v>1</v>
+      </c>
+      <c r="C72" t="s">
+        <v>2</v>
+      </c>
+      <c r="D72" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
App site's name changed and runners class fixed
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/resource/ScenarioStatus.xlsx
+++ b/src/test/java/ApachePOI/resource/ScenarioStatus.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="29">
   <si>
     <t>Create a country</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>Creating Country</t>
+  </si>
+  <si>
+    <t>27.12.22</t>
   </si>
 </sst>
 </file>
@@ -456,7 +459,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D98"/>
+  <dimension ref="A1:D118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
@@ -1840,6 +1843,286 @@
         <v>24</v>
       </c>
     </row>
+    <row r="99">
+      <c r="A99" t="s">
+        <v>25</v>
+      </c>
+      <c r="B99" t="s">
+        <v>5</v>
+      </c>
+      <c r="C99" t="s">
+        <v>2</v>
+      </c>
+      <c r="D99" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s">
+        <v>26</v>
+      </c>
+      <c r="B100" t="s">
+        <v>5</v>
+      </c>
+      <c r="C100" t="s">
+        <v>2</v>
+      </c>
+      <c r="D100" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s">
+        <v>20</v>
+      </c>
+      <c r="B101" t="s">
+        <v>5</v>
+      </c>
+      <c r="C101" t="s">
+        <v>2</v>
+      </c>
+      <c r="D101" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="s">
+        <v>20</v>
+      </c>
+      <c r="B102" t="s">
+        <v>5</v>
+      </c>
+      <c r="C102" t="s">
+        <v>2</v>
+      </c>
+      <c r="D102" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="s">
+        <v>20</v>
+      </c>
+      <c r="B103" t="s">
+        <v>5</v>
+      </c>
+      <c r="C103" t="s">
+        <v>2</v>
+      </c>
+      <c r="D103" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s">
+        <v>20</v>
+      </c>
+      <c r="B104" t="s">
+        <v>1</v>
+      </c>
+      <c r="C104" t="s">
+        <v>2</v>
+      </c>
+      <c r="D104" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s">
+        <v>25</v>
+      </c>
+      <c r="B105" t="s">
+        <v>1</v>
+      </c>
+      <c r="C105" t="s">
+        <v>2</v>
+      </c>
+      <c r="D105" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s">
+        <v>26</v>
+      </c>
+      <c r="B106" t="s">
+        <v>1</v>
+      </c>
+      <c r="C106" t="s">
+        <v>2</v>
+      </c>
+      <c r="D106" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s">
+        <v>25</v>
+      </c>
+      <c r="B107" t="s">
+        <v>1</v>
+      </c>
+      <c r="C107" t="s">
+        <v>2</v>
+      </c>
+      <c r="D107" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="s">
+        <v>26</v>
+      </c>
+      <c r="B108" t="s">
+        <v>5</v>
+      </c>
+      <c r="C108" t="s">
+        <v>2</v>
+      </c>
+      <c r="D108" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="s">
+        <v>25</v>
+      </c>
+      <c r="B109" t="s">
+        <v>1</v>
+      </c>
+      <c r="C109" t="s">
+        <v>9</v>
+      </c>
+      <c r="D109" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="s">
+        <v>26</v>
+      </c>
+      <c r="B110" t="s">
+        <v>1</v>
+      </c>
+      <c r="C110" t="s">
+        <v>9</v>
+      </c>
+      <c r="D110" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="s">
+        <v>25</v>
+      </c>
+      <c r="B111" t="s">
+        <v>1</v>
+      </c>
+      <c r="C111" t="s">
+        <v>2</v>
+      </c>
+      <c r="D111" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="s">
+        <v>25</v>
+      </c>
+      <c r="B112" t="s">
+        <v>1</v>
+      </c>
+      <c r="C112" t="s">
+        <v>9</v>
+      </c>
+      <c r="D112" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="s">
+        <v>26</v>
+      </c>
+      <c r="B113" t="s">
+        <v>5</v>
+      </c>
+      <c r="C113" t="s">
+        <v>2</v>
+      </c>
+      <c r="D113" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="s">
+        <v>26</v>
+      </c>
+      <c r="B114" t="s">
+        <v>5</v>
+      </c>
+      <c r="C114" t="s">
+        <v>9</v>
+      </c>
+      <c r="D114" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="s">
+        <v>25</v>
+      </c>
+      <c r="B115" t="s">
+        <v>1</v>
+      </c>
+      <c r="C115" t="s">
+        <v>2</v>
+      </c>
+      <c r="D115" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="s">
+        <v>25</v>
+      </c>
+      <c r="B116" t="s">
+        <v>1</v>
+      </c>
+      <c r="C116" t="s">
+        <v>9</v>
+      </c>
+      <c r="D116" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="s">
+        <v>26</v>
+      </c>
+      <c r="B117" t="s">
+        <v>1</v>
+      </c>
+      <c r="C117" t="s">
+        <v>2</v>
+      </c>
+      <c r="D117" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="s">
+        <v>26</v>
+      </c>
+      <c r="B118" t="s">
+        <v>1</v>
+      </c>
+      <c r="C118" t="s">
+        <v>9</v>
+      </c>
+      <c r="D118" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>